<commit_message>
adding front end and backend code
</commit_message>
<xml_diff>
--- a/sfChecker/output/AI_Service_Cloud_Capability_Report.xlsx
+++ b/sfChecker/output/AI_Service_Cloud_Capability_Report.xlsx
@@ -17,13 +17,16 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -34,7 +37,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -42,12 +45,21 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -413,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C51"/>
+  <dimension ref="A1:B49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -422,17 +434,12 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr">
         <is>
           <t>Capability Name</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Description</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>Enabled (YES/NO)</t>
         </is>
@@ -446,11 +453,6 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Central system to create, track, and resolve customer support cases.</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
           <t>YES</t>
         </is>
       </c>
@@ -463,11 +465,6 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Automatically route cases to</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
           <t>YES</t>
         </is>
       </c>
@@ -475,11 +472,10 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>agents or queues based on conditions.</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr"/>
-      <c r="C4" t="inlineStr">
+          <t>Escalation Rules</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
@@ -488,15 +484,10 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Escalation Rules</t>
+          <t>Auto Response Rules</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
-        <is>
-          <t>Escalate cases</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
@@ -505,11 +496,10 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>based on SLA breaches or priority conditions.</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr"/>
-      <c r="C6" t="inlineStr">
+          <t>Omni</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
@@ -518,32 +508,22 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Auto Response Rules</t>
+          <t>Entitlements</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Send automated email responses when cases are created.</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>NO</t>
+          <t>YES</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Omni</t>
+          <t>Milestones</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
-        <is>
-          <t>Channel Routing - Distribute work items to agents based on availability and skills.</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
@@ -552,15 +532,10 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Entitlements</t>
+          <t>Knowledge Base</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
-        <is>
-          <t>Define service agreements and support terms for customers.</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
@@ -569,15 +544,10 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Milestones</t>
+          <t>Email</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
-        <is>
-          <t>Track time-bound steps in service processes.</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
@@ -586,15 +556,10 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Knowledge Base</t>
+          <t>Web</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
-        <is>
-          <t>Central repository of articles for customer self-service and agents.</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
@@ -603,15 +568,10 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Email</t>
+          <t>Macros</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
-        <is>
-          <t>to-Case - Convert incoming emails into support cases automatically.</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
@@ -620,15 +580,10 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Web</t>
+          <t>Quick Text</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
-        <is>
-          <t>to-Case - Create cases from website forms submitted by customers.</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
@@ -637,15 +592,10 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Macros</t>
+          <t>Service Console</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
-        <is>
-          <t>Automations for repetitive tasks executed by support agents.</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
@@ -654,15 +604,10 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Quick Text</t>
+          <t>Live Chat</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
-        <is>
-          <t>Predefined text snippets for faster customer communication.</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
@@ -671,15 +616,10 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Service Console</t>
+          <t>CTI Integration</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
-        <is>
-          <t>Unified workspace interface for service agents.</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
@@ -688,15 +628,10 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Live Chat</t>
+          <t>Field Service Management</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
-        <is>
-          <t>Real-time chat support for customer interactions.</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
@@ -705,15 +640,10 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>CTI Integration</t>
+          <t>Einstein Bots</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
-        <is>
-          <t>Integrate telephony systems for call handling in Salesforce.</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
@@ -722,49 +652,34 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Field Service Management</t>
+          <t>Case Queues</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Manage field technicians, work orders, and on-site service.</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>NO</t>
+          <t>YES</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Einstein Bots</t>
+          <t>Service Level Agreements(SLAs)</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>AI chatbots for automated customer interactions.</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>NO</t>
+          <t>YES</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Case Queues</t>
+          <t>Reports</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
-        <is>
-          <t>Group cases for assignment to teams or departments.</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr">
         <is>
           <t>YES</t>
         </is>
@@ -773,32 +688,22 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Service Level Agreements(SLAs)</t>
+          <t>Dashboards</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Define service commitments and response timelines.</t>
-        </is>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>NO</t>
+          <t>YES</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Reports</t>
+          <t>Automation Flows</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
-        <is>
-          <t>Analytical views of service performance and operations.</t>
-        </is>
-      </c>
-      <c r="C23" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
@@ -807,15 +712,10 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Dashboards</t>
+          <t>Apex Triggers</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
-        <is>
-          <t>Visual metrics and KPIs for service operations. Automation Flows -</t>
-        </is>
-      </c>
-      <c r="C24" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
@@ -824,11 +724,10 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Workflow automation using Flow Builder.</t>
-        </is>
-      </c>
-      <c r="B25" t="inlineStr"/>
-      <c r="C25" t="inlineStr">
+          <t>API Integrations</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
@@ -837,15 +736,10 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Apex Triggers</t>
+          <t>Data Storage Monitoring</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
-        <is>
-          <t>Custom event-driven logic for automation.</t>
-        </is>
-      </c>
-      <c r="C26" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
@@ -854,15 +748,10 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>API Integrations</t>
+          <t>Permission Sets</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
-        <is>
-          <t>Integrate Salesforce with external applications and systems.</t>
-        </is>
-      </c>
-      <c r="C27" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
@@ -871,15 +760,10 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Data Storage Monitoring</t>
+          <t>Profiles</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
-        <is>
-          <t>Track data storage consumption and performance impact.</t>
-        </is>
-      </c>
-      <c r="C28" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
@@ -888,15 +772,10 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Permission Sets</t>
+          <t>Service Contracts</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
-        <is>
-          <t>Granular access control for users.</t>
-        </is>
-      </c>
-      <c r="C29" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
@@ -905,15 +784,10 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Profiles</t>
+          <t>Customer Community</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
-        <is>
-          <t>Role-based security configuration and permissions.</t>
-        </is>
-      </c>
-      <c r="C30" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
@@ -922,15 +796,10 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Service Contracts</t>
+          <t>Partner Community</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
-        <is>
-          <t>Manage long-term service agreements with customers.</t>
-        </is>
-      </c>
-      <c r="C31" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
@@ -939,15 +808,10 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Customer Community</t>
+          <t>Incident Management</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
-        <is>
-          <t>Self-service portals for customers.</t>
-        </is>
-      </c>
-      <c r="C32" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
@@ -956,15 +820,10 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Partner Community</t>
+          <t>Problem Management</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
-        <is>
-          <t>Support portals for partners.</t>
-        </is>
-      </c>
-      <c r="C33" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
@@ -973,15 +832,10 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Incident Management</t>
+          <t>Change Management</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
-        <is>
-          <t>Track major incidents affecting customers.</t>
-        </is>
-      </c>
-      <c r="C34" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
@@ -990,15 +844,10 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Problem Management</t>
+          <t>Asset Management</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
-        <is>
-          <t>Identify and resolve root causes of recurring issues.</t>
-        </is>
-      </c>
-      <c r="C35" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
@@ -1007,15 +856,10 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Change Management</t>
+          <t>Work Orders</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
-        <is>
-          <t>Manage updates and system changes affecting service.</t>
-        </is>
-      </c>
-      <c r="C36" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
@@ -1024,15 +868,10 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Asset Management</t>
+          <t>Service Appointments</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
-        <is>
-          <t>Track customer-owned products for support.</t>
-        </is>
-      </c>
-      <c r="C37" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
@@ -1041,15 +880,10 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Work Orders</t>
+          <t>Routing Configurations</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
-        <is>
-          <t>Manage service tasks for field operations.</t>
-        </is>
-      </c>
-      <c r="C38" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
@@ -1058,15 +892,10 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Service Appointments</t>
+          <t>Skills</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
-        <is>
-          <t>Schedule field service visits. Routing</t>
-        </is>
-      </c>
-      <c r="C39" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
@@ -1075,15 +904,10 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Configurations</t>
+          <t>Presence Configurations</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
-        <is>
-          <t>Define logic for routing work items. Skills-Based</t>
-        </is>
-      </c>
-      <c r="C40" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
@@ -1092,15 +916,10 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Routing</t>
+          <t>Social Customer Service</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
-        <is>
-          <t>Assign work based on agent expertise. Presence</t>
-        </is>
-      </c>
-      <c r="C41" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
@@ -1109,15 +928,10 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Configurations</t>
+          <t>Messaging Channels</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
-        <is>
-          <t>Manage agent availability status. Social Customer</t>
-        </is>
-      </c>
-      <c r="C42" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
@@ -1126,32 +940,22 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Service</t>
+          <t>Case Swarming</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Support customers through social media channels. Messaging</t>
-        </is>
-      </c>
-      <c r="C43" t="inlineStr">
-        <is>
-          <t>NO</t>
+          <t>YES</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Channels</t>
+          <t>Service Analytics</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
-        <is>
-          <t>Support via WhatsApp, SMS, and messaging apps. Case</t>
-        </is>
-      </c>
-      <c r="C44" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
@@ -1160,15 +964,10 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Swarming</t>
+          <t>Customer Feedback Surveys</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
-        <is>
-          <t>Collaborative case resolution among multiple agents. Service</t>
-        </is>
-      </c>
-      <c r="C45" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
@@ -1177,15 +976,10 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Analytics</t>
+          <t>Knowledge Recommendations</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
-        <is>
-          <t>Advanced analytics for service operations. Customer Feedback</t>
-        </is>
-      </c>
-      <c r="C46" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
@@ -1194,32 +988,22 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Surveys</t>
+          <t>Einstein Case Classification</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Collect customer satisfaction data. Knowledge</t>
-        </is>
-      </c>
-      <c r="C47" t="inlineStr">
-        <is>
-          <t>NO</t>
+          <t>YES</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Recommendations</t>
+          <t>Einstein Next Best Action</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
-        <is>
-          <t>Suggest relevant articles during case handling.</t>
-        </is>
-      </c>
-      <c r="C48" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
@@ -1228,49 +1012,10 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Einstein Case Classification</t>
+          <t>Service Forecasting</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
-        <is>
-          <t>AI-driven case categorization. Einstein</t>
-        </is>
-      </c>
-      <c r="C49" t="inlineStr">
-        <is>
-          <t>YES</t>
-        </is>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" t="inlineStr">
-        <is>
-          <t>Next Best Action</t>
-        </is>
-      </c>
-      <c r="B50" t="inlineStr">
-        <is>
-          <t>Recommend actions for agents during service. Service</t>
-        </is>
-      </c>
-      <c r="C50" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" t="inlineStr">
-        <is>
-          <t>Forecasting</t>
-        </is>
-      </c>
-      <c r="B51" t="inlineStr">
-        <is>
-          <t>Predict service demand and workload.</t>
-        </is>
-      </c>
-      <c r="C51" t="inlineStr">
         <is>
           <t>NO</t>
         </is>

</xml_diff>